<commit_message>
Sheet 'Eesti_KOV (2)'; Additional columns 'Viibimise maakond' and 'Viibimise vald/linn' in sheet 'Veerud + valikud'. Freeze Panes.
</commit_message>
<xml_diff>
--- a/downloads/ANDMED.xlsx
+++ b/downloads/ANDMED.xlsx
@@ -11,31 +11,58 @@
     <sheet name="Veerud + valikud" sheetId="1" r:id="rId2"/>
     <sheet name="Lists" sheetId="3" r:id="rId3"/>
     <sheet name="Eesti_KOV" sheetId="6" r:id="rId4"/>
-    <sheet name="Stuff" sheetId="5" r:id="rId5"/>
+    <sheet name="Eesti_KOV (2)" sheetId="7" r:id="rId5"/>
+    <sheet name="Names" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="Eesti_KOV_2_Maakond">Eesti_KOV_2[#Headers]</definedName>
+    <definedName name="Eesti_KOV_Maakond_Vald_Linn" localSheetId="4">#REF!</definedName>
     <definedName name="Eesti_KOV_Maakond_Vald_Linn">Eesti_KOV[Maakond+Vald/Linn]</definedName>
-    <definedName name="Last_Update">README!$B$12</definedName>
+    <definedName name="Harju_maakond">'Eesti_KOV (2)'!$A$2:$A$17</definedName>
+    <definedName name="Hiiu_maakond">'Eesti_KOV (2)'!$B$2:$B$17</definedName>
+    <definedName name="Ida_Viru_maakond">'Eesti_KOV (2)'!$C$2:$C$17</definedName>
+    <definedName name="Jõgeva_maakond">'Eesti_KOV (2)'!$D$2:$D$17</definedName>
+    <definedName name="Järva_maakond">'Eesti_KOV (2)'!$E$2:$E$17</definedName>
+    <definedName name="Last_Update">README!$B$15</definedName>
+    <definedName name="Lists_Elukutse" localSheetId="4">Elukutse[Elukutse]</definedName>
     <definedName name="Lists_Elukutse">Elukutse[Elukutse]</definedName>
+    <definedName name="Lists_Kontakti_koht" localSheetId="4">Kontakti_koht[Kontakti koht]</definedName>
     <definedName name="Lists_Kontakti_koht">Kontakti_koht[Kontakti koht]</definedName>
+    <definedName name="Lists_Kontakti_tüüp" localSheetId="4">Kontakti_tüüp[Kontakti tüüp]</definedName>
     <definedName name="Lists_Kontakti_tüüp">Kontakti_tüüp[Kontakti tüüp]</definedName>
+    <definedName name="Lists_Peamised_sümptomid" localSheetId="4">Peamised_sümptomid[Peamised sümptomid]</definedName>
     <definedName name="Lists_Peamised_sümptomid">Peamised_sümptomid[Peamised sümptomid]</definedName>
+    <definedName name="Lists_Riskipiirkonnas_viibimine" localSheetId="4">Riskipiirkonnas_viibimine[Riskipiirkonnas viibimine]</definedName>
     <definedName name="Lists_Riskipiirkonnas_viibimine">Riskipiirkonnas_viibimine[Riskipiirkonnas viibimine]</definedName>
+    <definedName name="Lists_Sugu" localSheetId="4">Sugu[Sugu]</definedName>
     <definedName name="Lists_Sugu">Sugu[Sugu]</definedName>
+    <definedName name="Lists_Tulemus" localSheetId="4">Tulemus[Tulemus]</definedName>
     <definedName name="Lists_Tulemus">Tulemus[Tulemus]</definedName>
-    <definedName name="Maximum_Eestisse_saabumise_kpv">Stuff!$B$5</definedName>
-    <definedName name="Maximum_Esimeste_haigusnähtude_ilmumise_kuupäev">Stuff!$B$7</definedName>
-    <definedName name="Maximum_Jälgimise_kuupäev">Stuff!$B$11</definedName>
-    <definedName name="Maximum_Kontakti_viimane_kpv">Stuff!$B$3</definedName>
-    <definedName name="Maximum_Temperatuur">Stuff!$B$9</definedName>
-    <definedName name="Minimum_Eestisse_saabumise_kpv">Stuff!$B$4</definedName>
-    <definedName name="Minimum_Esimeste_haigusnähtude_ilmumise_kuupäev">Stuff!$B$6</definedName>
-    <definedName name="Minimum_Jälgimise_kuupäev">Stuff!$B$10</definedName>
-    <definedName name="Minimum_Kontakti_viimane_kpv">Stuff!$B$2</definedName>
-    <definedName name="Minimum_Temperatuur">Stuff!$B$8</definedName>
-    <definedName name="TrueBlank">Stuff!$B$1</definedName>
+    <definedName name="Lääne_maakond">'Eesti_KOV (2)'!$F$2:$F$17</definedName>
+    <definedName name="Lääne_Viru_maakond">'Eesti_KOV (2)'!$G$2:$G$17</definedName>
+    <definedName name="Maximum_Eestisse_saabumise_kpv">Names!$B$5</definedName>
+    <definedName name="Maximum_Esimeste_haigusnähtude_ilmumise_kuupäev">Names!$B$7</definedName>
+    <definedName name="Maximum_Jälgimise_kuupäev">Names!$B$11</definedName>
+    <definedName name="Maximum_Kontakti_viimane_kpv">Names!$B$3</definedName>
+    <definedName name="Maximum_Temperatuur">Names!$B$9</definedName>
+    <definedName name="Minimum_Eestisse_saabumise_kpv">Names!$B$4</definedName>
+    <definedName name="Minimum_Esimeste_haigusnähtude_ilmumise_kuupäev">Names!$B$6</definedName>
+    <definedName name="Minimum_Jälgimise_kuupäev">Names!$B$10</definedName>
+    <definedName name="Minimum_Kontakti_viimane_kpv">Names!$B$2</definedName>
+    <definedName name="Minimum_Temperatuur">Names!$B$8</definedName>
+    <definedName name="Põlva_maakond">'Eesti_KOV (2)'!$H$2:$H$17</definedName>
+    <definedName name="Pärnu_maakond">'Eesti_KOV (2)'!$I$2:$I$17</definedName>
+    <definedName name="Rapla_maakond">'Eesti_KOV (2)'!$J$2:$J$17</definedName>
+    <definedName name="Saare_maakond">'Eesti_KOV (2)'!$K$2:$K$17</definedName>
+    <definedName name="Tartu_maakond">'Eesti_KOV (2)'!$L$2:$L$17</definedName>
+    <definedName name="TrueBlank">Names!$B$1</definedName>
+    <definedName name="Username_Authors" localSheetId="4">Authors[Username]</definedName>
     <definedName name="Username_Authors">Authors[Username]</definedName>
+    <definedName name="Valga_maakond">'Eesti_KOV (2)'!$M$2:$M$17</definedName>
+    <definedName name="When_Changes" localSheetId="4">Changes[When]</definedName>
     <definedName name="When_Changes">Changes[When]</definedName>
+    <definedName name="Viljandi_maakond">'Eesti_KOV (2)'!$N$2:$N$17</definedName>
+    <definedName name="Võru_maakond">'Eesti_KOV (2)'!$O$2:$O$17</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -76,12 +103,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="D2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Can be deleted or hidden in case separate columns 'Viibimise maakond' and 'Viibimise vald/linn' are kept together with sheet 'Eesti KOV (2)'</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="267">
   <si>
     <t>2) Ekspositsioon ja reisimine</t>
   </si>
@@ -858,6 +909,30 @@
   </si>
   <si>
     <t>Sheet 'Eesti_KOV' and data validation in sheet 'Veerud + valikud' column 'Viibimise maakond/linn'</t>
+  </si>
+  <si>
+    <t>Viibimise maakond</t>
+  </si>
+  <si>
+    <t>Viibimise vald/linn</t>
+  </si>
+  <si>
+    <t>https://github.com/okestonia/opendata.riik.ee/commit/eb315d36a84f00a3bae19a54159399774de3d068</t>
+  </si>
+  <si>
+    <t>keeganmcbride</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Source Eesti_KOV (2)</t>
+  </si>
+  <si>
+    <t>Suggested to be used as template by Terviseamet to publish near-real-time CSV-data as opendata for data analysis</t>
+  </si>
+  <si>
+    <t>Sheet 'Eesti_KOV (2)'; Additional columns 'Viibimise maakond' and 'Viibimise vald/linn' in sheet 'Veerud + valikud'. Freeze Panes.</t>
   </si>
 </sst>
 </file>
@@ -867,7 +942,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -935,6 +1010,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1134,7 +1227,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
@@ -1254,6 +1347,7 @@
     <xf numFmtId="22" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="22" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1266,24 +1360,6 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1331,19 +1407,6 @@
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1376,11 +1439,7 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1391,6 +1450,41 @@
           <color indexed="64"/>
         </right>
       </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1406,8 +1500,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Changes" displayName="Changes" ref="B15:D20" totalsRowShown="0">
-  <autoFilter ref="B15:D20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Changes" displayName="Changes" ref="B18:D25" totalsRowShown="0">
+  <autoFilter ref="B18:D25"/>
   <tableColumns count="3">
     <tableColumn id="1" name="When"/>
     <tableColumn id="2" name="Who"/>
@@ -1433,7 +1527,7 @@
   <tableColumns count="3">
     <tableColumn id="1" name="Maakond"/>
     <tableColumn id="2" name="Vald/Linn"/>
-    <tableColumn id="3" name="Maakond+Vald/Linn" dataDxfId="2">
+    <tableColumn id="3" name="Maakond+Vald/Linn" dataDxfId="1">
       <calculatedColumnFormula>Eesti_KOV[[#This Row],[Maakond]]&amp;" - "&amp;Eesti_KOV[[#This Row],[Vald/Linn]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1441,11 +1535,35 @@
 </table>
 </file>
 
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Eesti_KOV_2" displayName="Eesti_KOV_2" ref="A1:O17" totalsRowShown="0">
+  <autoFilter ref="A1:O17"/>
+  <tableColumns count="15">
+    <tableColumn id="1" name="Harju maakond"/>
+    <tableColumn id="2" name="Hiiu maakond"/>
+    <tableColumn id="3" name="Ida-Viru maakond"/>
+    <tableColumn id="4" name="Jõgeva maakond"/>
+    <tableColumn id="5" name="Järva maakond"/>
+    <tableColumn id="6" name="Lääne maakond"/>
+    <tableColumn id="7" name="Lääne-Viru maakond"/>
+    <tableColumn id="8" name="Põlva maakond"/>
+    <tableColumn id="9" name="Pärnu maakond"/>
+    <tableColumn id="10" name="Rapla maakond"/>
+    <tableColumn id="11" name="Saare maakond"/>
+    <tableColumn id="12" name="Tartu maakond"/>
+    <tableColumn id="13" name="Valga maakond"/>
+    <tableColumn id="14" name="Viljandi maakond"/>
+    <tableColumn id="15" name="Võru maakond"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Authors" displayName="Authors" ref="B7:E9" totalsRowShown="0">
-  <autoFilter ref="B7:E9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Authors" displayName="Authors" ref="B9:E12" totalsRowShown="0">
+  <autoFilter ref="B9:E12"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Username" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" name="Username" dataDxfId="23" dataCellStyle="Hyperlink"/>
     <tableColumn id="2" name="Fisrtname Lastname"/>
     <tableColumn id="3" name="Email"/>
     <tableColumn id="4" name="Phone"/>
@@ -1455,21 +1573,23 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="B2:BG17" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="22" tableBorderDxfId="23">
-  <autoFilter ref="B2:BG17"/>
-  <tableColumns count="58">
-    <tableColumn id="1" name="Unikaalne number " dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="B2:BI17" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20">
+  <autoFilter ref="B2:BI17"/>
+  <tableColumns count="60">
+    <tableColumn id="1" name="Unikaalne number " dataDxfId="19">
       <calculatedColumnFormula>ROW()-2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="N.A."/>
     <tableColumn id="3" name="Viibimise maakond/linn"/>
+    <tableColumn id="60" name="Viibimise maakond"/>
+    <tableColumn id="59" name="Viibimise vald/linn"/>
     <tableColumn id="4" name="Aadress (elukoht)"/>
     <tableColumn id="5" name="Eesnimi perekonnanimi"/>
     <tableColumn id="6" name="Sugu"/>
     <tableColumn id="7" name="Vanus"/>
     <tableColumn id="8" name="E-post"/>
     <tableColumn id="9" name="Telefoni nr"/>
-    <tableColumn id="10" name="Kontakti tüüp" dataDxfId="21"/>
+    <tableColumn id="10" name="Kontakti tüüp" dataDxfId="18"/>
     <tableColumn id="11" name="N.A.2"/>
     <tableColumn id="12" name="Kontakti koht"/>
     <tableColumn id="13" name="Kontakti koha täpsustus"/>
@@ -1479,7 +1599,7 @@
     <tableColumn id="17" name="Reisiinfo (tagasiulatuv kuni 14 päeva kohta enne sümptomite avaldumist) - riigid"/>
     <tableColumn id="18" name="Eestisse saabumise teekond"/>
     <tableColumn id="19" name="Eestisse saabumise kpv"/>
-    <tableColumn id="20" name="N.A.3" dataDxfId="20"/>
+    <tableColumn id="20" name="N.A.3" dataDxfId="17"/>
     <tableColumn id="21" name="N.A.4"/>
     <tableColumn id="22" name="N.A.5"/>
     <tableColumn id="23" name="N.A.6"/>
@@ -1487,60 +1607,60 @@
     <tableColumn id="25" name="N.A.8"/>
     <tableColumn id="26" name="N.A.9"/>
     <tableColumn id="27" name="Esimeste haigusnähtude ilmumise kuupäev"/>
-    <tableColumn id="28" name="Peamised sümptomid" dataDxfId="19"/>
+    <tableColumn id="28" name="Peamised sümptomid" dataDxfId="16"/>
     <tableColumn id="29" name="Temperatuur"/>
     <tableColumn id="30" name="N.A.10"/>
-    <tableColumn id="31" name="kuupäev_01" dataDxfId="16"/>
+    <tableColumn id="31" name="kuupäev_01" dataDxfId="15"/>
     <tableColumn id="32" name="tulemus_01"/>
-    <tableColumn id="33" name="kuupäev_02" dataDxfId="15">
+    <tableColumn id="33" name="kuupäev_02" dataDxfId="14">
       <calculatedColumnFormula>IF(AND(Table8[[#This Row],[tulemus_01]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_01]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_01]]+1,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="34" name="tulemus_02"/>
-    <tableColumn id="35" name="kuupäev_03" dataDxfId="14">
+    <tableColumn id="35" name="kuupäev_03" dataDxfId="13">
       <calculatedColumnFormula>IF(AND(Table8[[#This Row],[tulemus_02]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_02]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_02]]+1,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="36" name="tulemus_03"/>
-    <tableColumn id="37" name="kuupäev_04" dataDxfId="13">
+    <tableColumn id="37" name="kuupäev_04" dataDxfId="12">
       <calculatedColumnFormula>IF(AND(Table8[[#This Row],[tulemus_03]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_03]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_03]]+1,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="38" name="tulemus_04"/>
-    <tableColumn id="39" name="kuupäev_05" dataDxfId="12">
+    <tableColumn id="39" name="kuupäev_05" dataDxfId="11">
       <calculatedColumnFormula>IF(AND(Table8[[#This Row],[tulemus_04]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_04]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_04]]+1,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="40" name="tulemus_05"/>
-    <tableColumn id="41" name="kuupäev_06" dataDxfId="11">
+    <tableColumn id="41" name="kuupäev_06" dataDxfId="10">
       <calculatedColumnFormula>IF(AND(Table8[[#This Row],[tulemus_05]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_05]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_05]]+1,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="42" name="tulemus_06"/>
-    <tableColumn id="43" name="kuupäev_07" dataDxfId="10">
+    <tableColumn id="43" name="kuupäev_07" dataDxfId="9">
       <calculatedColumnFormula>IF(AND(Table8[[#This Row],[tulemus_06]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_06]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_06]]+1,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="44" name="tulemus_07"/>
-    <tableColumn id="45" name="kuupäev_08" dataDxfId="9">
+    <tableColumn id="45" name="kuupäev_08" dataDxfId="8">
       <calculatedColumnFormula>IF(AND(Table8[[#This Row],[tulemus_07]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_07]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_07]]+1,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="46" name="tulemus_08"/>
-    <tableColumn id="47" name="kuupäev_09" dataDxfId="8">
+    <tableColumn id="47" name="kuupäev_09" dataDxfId="7">
       <calculatedColumnFormula>IF(AND(Table8[[#This Row],[tulemus_08]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_08]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_08]]+1,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="48" name="tulemus_09"/>
-    <tableColumn id="49" name="kuupäev_10" dataDxfId="7">
+    <tableColumn id="49" name="kuupäev_10" dataDxfId="6">
       <calculatedColumnFormula>IF(AND(Table8[[#This Row],[tulemus_09]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_09]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_09]]+1,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="50" name="tulemus_10"/>
-    <tableColumn id="51" name="kuupäev_11" dataDxfId="6">
+    <tableColumn id="51" name="kuupäev_11" dataDxfId="5">
       <calculatedColumnFormula>IF(AND(Table8[[#This Row],[tulemus_10]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_10]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_10]]+1,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="52" name="tulemus_11"/>
-    <tableColumn id="53" name="kuupäev_12" dataDxfId="5">
+    <tableColumn id="53" name="kuupäev_12" dataDxfId="4">
       <calculatedColumnFormula>IF(AND(Table8[[#This Row],[tulemus_11]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_11]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_11]]+1,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="54" name="tulemus_12"/>
-    <tableColumn id="55" name="kuupäev_13" dataDxfId="4">
+    <tableColumn id="55" name="kuupäev_13" dataDxfId="3">
       <calculatedColumnFormula>IF(AND(Table8[[#This Row],[tulemus_12]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_12]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_12]]+1,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="56" name="tulemus_13"/>
-    <tableColumn id="57" name="kuupäev_14" dataDxfId="3">
+    <tableColumn id="57" name="kuupäev_14" dataDxfId="2">
       <calculatedColumnFormula>IF(AND(Table8[[#This Row],[tulemus_13]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_13]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_13]]+1,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="58" name="tulemus_14"/>
@@ -1872,10 +1992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1895,187 +2015,231 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>101</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" s="32">
-        <v>43904.833333333336</v>
+        <v>100</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="32">
+        <v>43904.833333333336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>254</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B6" s="44" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="44"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>264</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="44"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>152</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B9" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
         <v>154</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D9" t="s">
         <v>155</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E9" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="46" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="47" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C11" t="s">
         <v>149</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D11" t="s">
         <v>150</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E11" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="46"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="44"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="43" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="46"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="44"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="43" t="s">
         <v>255</v>
       </c>
-      <c r="B12" s="33">
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="33">
         <f>MAX(When_Changes)</f>
-        <v>43904.916666666664</v>
-      </c>
-      <c r="C12" s="34" t="str">
+        <v>43905.375</v>
+      </c>
+      <c r="C15" s="34" t="str">
         <f>INDEX(Changes[Who],MATCH(Last_Update,Changes[When],0))</f>
         <v>toomasm</v>
       </c>
-      <c r="D12" s="35" t="str">
+      <c r="D15" s="35" t="str">
         <f>INDEX(Changes[What],MATCH(Last_Update,Changes[When],0))</f>
-        <v>Sheet 'Eesti_KOV' and data validation in sheet 'Veerud + valikud' column 'Viibimise maakond/linn'</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+        <v>Sheet 'Eesti_KOV (2)'; Additional columns 'Viibimise maakond' and 'Viibimise vald/linn' in sheet 'Veerud + valikud'. Freeze Panes.</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" t="s">
         <v>106</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C18" t="s">
         <v>105</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D18" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B16" s="32">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="32">
+        <v>43904.412499999999</v>
+      </c>
+      <c r="C19" t="s">
+        <v>262</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="32">
         <v>43904.829861111109</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C20" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D20" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="32">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="32">
         <v>43904.833333333336</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C21" t="s">
         <v>108</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D21" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="32">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="32">
         <v>43904.836805555555</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C22" t="s">
         <v>108</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D22" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="32">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="32">
         <v>43904.902777777781</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C23" t="s">
         <v>108</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D23" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="32">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="32">
         <v>43904.916666666664</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C24" t="s">
         <v>108</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D24" t="s">
         <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="32">
+        <v>43905.375</v>
+      </c>
+      <c r="C25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16:C20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:C25">
       <formula1>Username_Authors</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="D19" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
   <tableParts count="2">
-    <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:BM18"/>
+  <dimension ref="B1:BO18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AB3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2103,7 +2267,7 @@
     <col min="32" max="32" width="10.7109375" customWidth="1"/>
     <col min="33" max="33" width="39.7109375" customWidth="1"/>
     <col min="34" max="34" width="12.7109375" customWidth="1"/>
-    <col min="35" max="35" width="12.42578125" customWidth="1"/>
+    <col min="35" max="35" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="12.7109375" customWidth="1"/>
     <col min="37" max="37" width="12.42578125" customWidth="1"/>
     <col min="38" max="38" width="12.7109375" customWidth="1"/>
@@ -2131,7 +2295,7 @@
     <col min="60" max="60" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:65" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:67" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="29" t="s">
         <v>79</v>
       </c>
@@ -2143,91 +2307,93 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="6"/>
       <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
       <c r="R1" s="7"/>
       <c r="S1" s="7"/>
       <c r="T1" s="7"/>
-      <c r="U1" s="29" t="s">
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="1"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="2"/>
       <c r="Z1" s="3"/>
-      <c r="AA1" s="8"/>
+      <c r="AA1" s="3"/>
       <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="9" t="s">
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="10" t="s">
+      <c r="AH1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="AG1" s="11"/>
-      <c r="AH1" s="12" t="s">
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="10" t="s">
+      <c r="AK1" s="13"/>
+      <c r="AL1" s="10" t="s">
         <v>5</v>
-      </c>
-      <c r="AK1" s="11"/>
-      <c r="AL1" s="10" t="s">
-        <v>6</v>
       </c>
       <c r="AM1" s="11"/>
       <c r="AN1" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AO1" s="11"/>
       <c r="AP1" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AQ1" s="11"/>
       <c r="AR1" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AS1" s="11"/>
       <c r="AT1" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AU1" s="11"/>
       <c r="AV1" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AW1" s="11"/>
       <c r="AX1" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AY1" s="11"/>
       <c r="AZ1" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="BA1" s="11"/>
       <c r="BB1" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="BC1" s="11"/>
       <c r="BD1" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="BE1" s="11"/>
       <c r="BF1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="BG1" s="11"/>
+      <c r="BH1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="BG1" s="11"/>
-    </row>
-    <row r="2" spans="2:65" s="14" customFormat="1" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BI1" s="11"/>
+    </row>
+    <row r="2" spans="2:67" s="14" customFormat="1" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="15" t="s">
         <v>80</v>
       </c>
@@ -2238,1283 +2404,1399 @@
         <v>34</v>
       </c>
       <c r="E2" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="H2" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="I2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="J2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="K2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="L2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="M2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="N2" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="O2" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="P2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="Q2" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="R2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="S2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="15" t="s">
+      <c r="T2" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="S2" s="15" t="s">
+      <c r="U2" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="V2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="30" t="s">
+      <c r="W2" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="V2" s="23" t="s">
+      <c r="X2" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="W2" s="23" t="s">
+      <c r="Y2" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="X2" s="23" t="s">
+      <c r="Z2" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="Y2" s="23" t="s">
+      <c r="AA2" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="Z2" s="23" t="s">
+      <c r="AB2" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="AA2" s="23" t="s">
+      <c r="AC2" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="AB2" s="16" t="s">
+      <c r="AD2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="16" t="s">
+      <c r="AE2" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="AD2" s="19" t="s">
+      <c r="AF2" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="AE2" s="22" t="s">
+      <c r="AG2" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="AF2" s="18" t="s">
+      <c r="AH2" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="AG2" s="15" t="s">
+      <c r="AI2" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="AH2" s="18" t="s">
+      <c r="AJ2" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="AI2" s="15" t="s">
+      <c r="AK2" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="AJ2" s="18" t="s">
+      <c r="AL2" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="AK2" s="15" t="s">
+      <c r="AM2" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="AL2" s="18" t="s">
+      <c r="AN2" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="AM2" s="15" t="s">
+      <c r="AO2" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="AN2" s="18" t="s">
+      <c r="AP2" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="AO2" s="15" t="s">
+      <c r="AQ2" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="AP2" s="18" t="s">
+      <c r="AR2" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="AQ2" s="15" t="s">
+      <c r="AS2" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="AR2" s="18" t="s">
+      <c r="AT2" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="AS2" s="15" t="s">
+      <c r="AU2" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="AT2" s="18" t="s">
+      <c r="AV2" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="AU2" s="15" t="s">
+      <c r="AW2" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="AV2" s="18" t="s">
+      <c r="AX2" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="AW2" s="15" t="s">
+      <c r="AY2" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="AX2" s="18" t="s">
+      <c r="AZ2" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="AY2" s="15" t="s">
+      <c r="BA2" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="AZ2" s="18" t="s">
+      <c r="BB2" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="BA2" s="15" t="s">
+      <c r="BC2" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="BB2" s="18" t="s">
+      <c r="BD2" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="BC2" s="15" t="s">
+      <c r="BE2" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="BD2" s="18" t="s">
+      <c r="BF2" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="BE2" s="15" t="s">
+      <c r="BG2" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="BF2" s="18" t="s">
+      <c r="BH2" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="BG2" s="15" t="s">
+      <c r="BI2" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="BH2" s="24"/>
-      <c r="BI2"/>
-      <c r="BJ2"/>
+      <c r="BJ2" s="24"/>
       <c r="BK2"/>
       <c r="BL2"/>
       <c r="BM2"/>
-    </row>
-    <row r="3" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="BN2"/>
+      <c r="BO2"/>
+    </row>
+    <row r="3" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B3" s="24">
         <f t="shared" ref="B3:B17" si="0">ROW()-2</f>
         <v>1</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>81</v>
       </c>
-      <c r="K3" s="28" t="s">
+      <c r="K3"/>
+      <c r="M3" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>43</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>73</v>
       </c>
-      <c r="P3" s="36"/>
-      <c r="Q3" t="s">
+      <c r="R3" s="36"/>
+      <c r="S3" t="s">
         <v>32</v>
       </c>
-      <c r="AC3" s="24" t="s">
+      <c r="U3"/>
+      <c r="W3" s="28"/>
+      <c r="AC3"/>
+      <c r="AD3"/>
+      <c r="AE3" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="AF3" s="36"/>
-      <c r="AG3" t="s">
+      <c r="AF3" s="24"/>
+      <c r="AH3" s="36"/>
+      <c r="AI3" t="s">
         <v>36</v>
       </c>
-      <c r="AH3" s="36" t="str">
+      <c r="AJ3" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_01]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_01]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_01]]+1,"")</f>
         <v/>
       </c>
-      <c r="AJ3" s="36" t="str">
+      <c r="AL3" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_02]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_02]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_02]]+1,"")</f>
         <v/>
       </c>
-      <c r="AL3" s="36" t="str">
+      <c r="AN3" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_03]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_03]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_03]]+1,"")</f>
         <v/>
       </c>
-      <c r="AN3" s="36" t="str">
+      <c r="AP3" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_04]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_04]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_04]]+1,"")</f>
         <v/>
       </c>
-      <c r="AP3" s="36" t="str">
+      <c r="AR3" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_05]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_05]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_05]]+1,"")</f>
         <v/>
       </c>
-      <c r="AR3" s="36" t="str">
+      <c r="AT3" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_06]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_06]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_06]]+1,"")</f>
         <v/>
       </c>
-      <c r="AT3" s="36" t="str">
+      <c r="AV3" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_07]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_07]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_07]]+1,"")</f>
         <v/>
       </c>
-      <c r="AV3" s="36" t="str">
+      <c r="AX3" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_08]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_08]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_08]]+1,"")</f>
         <v/>
       </c>
-      <c r="AX3" s="36" t="str">
+      <c r="AZ3" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_09]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_09]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_09]]+1,"")</f>
         <v/>
       </c>
-      <c r="AZ3" s="36" t="str">
+      <c r="BB3" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_10]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_10]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_10]]+1,"")</f>
         <v/>
       </c>
-      <c r="BB3" s="36" t="str">
+      <c r="BD3" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_11]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_11]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_11]]+1,"")</f>
         <v/>
       </c>
-      <c r="BD3" s="36" t="str">
+      <c r="BF3" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_12]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_12]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_12]]+1,"")</f>
         <v/>
       </c>
-      <c r="BF3" s="36" t="str">
+      <c r="BH3" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_13]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_13]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_13]]+1,"")</f>
         <v/>
       </c>
-      <c r="BH3" s="24"/>
-    </row>
-    <row r="4" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="BJ3" s="24"/>
+    </row>
+    <row r="4" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B4" s="24">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4"/>
+      <c r="M4" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>44</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>74</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>33</v>
       </c>
-      <c r="AC4" s="24" t="s">
+      <c r="U4"/>
+      <c r="W4" s="28"/>
+      <c r="AC4"/>
+      <c r="AD4"/>
+      <c r="AE4" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="AF4" s="36"/>
-      <c r="AG4" t="s">
+      <c r="AF4" s="24"/>
+      <c r="AH4" s="36"/>
+      <c r="AI4" t="s">
         <v>37</v>
       </c>
-      <c r="AH4" s="36" t="str">
+      <c r="AJ4" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_01]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_01]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_01]]+1,"")</f>
         <v/>
       </c>
-      <c r="AJ4" s="36" t="str">
+      <c r="AL4" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_02]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_02]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_02]]+1,"")</f>
         <v/>
       </c>
-      <c r="AL4" s="36" t="str">
+      <c r="AN4" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_03]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_03]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_03]]+1,"")</f>
         <v/>
       </c>
-      <c r="AN4" s="36" t="str">
+      <c r="AP4" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_04]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_04]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_04]]+1,"")</f>
         <v/>
       </c>
-      <c r="AP4" s="36" t="str">
+      <c r="AR4" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_05]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_05]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_05]]+1,"")</f>
         <v/>
       </c>
-      <c r="AR4" s="36" t="str">
+      <c r="AT4" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_06]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_06]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_06]]+1,"")</f>
         <v/>
       </c>
-      <c r="AT4" s="36" t="str">
+      <c r="AV4" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_07]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_07]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_07]]+1,"")</f>
         <v/>
       </c>
-      <c r="AV4" s="36" t="str">
+      <c r="AX4" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_08]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_08]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_08]]+1,"")</f>
         <v/>
       </c>
-      <c r="AX4" s="36" t="str">
+      <c r="AZ4" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_09]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_09]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_09]]+1,"")</f>
         <v/>
       </c>
-      <c r="AZ4" s="36" t="str">
+      <c r="BB4" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_10]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_10]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_10]]+1,"")</f>
         <v/>
       </c>
-      <c r="BB4" s="36" t="str">
+      <c r="BD4" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_11]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_11]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_11]]+1,"")</f>
         <v/>
       </c>
-      <c r="BD4" s="36" t="str">
+      <c r="BF4" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_12]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_12]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_12]]+1,"")</f>
         <v/>
       </c>
-      <c r="BF4" s="36" t="str">
+      <c r="BH4" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_13]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_13]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_13]]+1,"")</f>
         <v/>
       </c>
-      <c r="BH4" s="24"/>
-    </row>
-    <row r="5" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="BJ4" s="24"/>
+    </row>
+    <row r="5" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B5" s="24">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="M5" t="s">
+      <c r="K5"/>
+      <c r="M5" s="28"/>
+      <c r="O5" t="s">
         <v>84</v>
       </c>
-      <c r="O5" t="s">
+      <c r="Q5" t="s">
         <v>75</v>
       </c>
-      <c r="AC5" s="24" t="s">
+      <c r="U5"/>
+      <c r="W5" s="28"/>
+      <c r="AC5"/>
+      <c r="AD5"/>
+      <c r="AE5" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="AF5" s="36"/>
-      <c r="AG5" t="s">
+      <c r="AF5" s="24"/>
+      <c r="AH5" s="36"/>
+      <c r="AI5" t="s">
         <v>38</v>
       </c>
-      <c r="AH5" s="36" t="str">
+      <c r="AJ5" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_01]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_01]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_01]]+1,"")</f>
         <v/>
       </c>
-      <c r="AJ5" s="36" t="str">
+      <c r="AL5" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_02]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_02]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_02]]+1,"")</f>
         <v/>
       </c>
-      <c r="AL5" s="36" t="str">
+      <c r="AN5" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_03]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_03]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_03]]+1,"")</f>
         <v/>
       </c>
-      <c r="AN5" s="36" t="str">
+      <c r="AP5" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_04]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_04]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_04]]+1,"")</f>
         <v/>
       </c>
-      <c r="AP5" s="36" t="str">
+      <c r="AR5" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_05]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_05]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_05]]+1,"")</f>
         <v/>
       </c>
-      <c r="AR5" s="36" t="str">
+      <c r="AT5" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_06]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_06]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_06]]+1,"")</f>
         <v/>
       </c>
-      <c r="AT5" s="36" t="str">
+      <c r="AV5" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_07]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_07]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_07]]+1,"")</f>
         <v/>
       </c>
-      <c r="AV5" s="36" t="str">
+      <c r="AX5" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_08]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_08]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_08]]+1,"")</f>
         <v/>
       </c>
-      <c r="AX5" s="36" t="str">
+      <c r="AZ5" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_09]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_09]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_09]]+1,"")</f>
         <v/>
       </c>
-      <c r="AZ5" s="36" t="str">
+      <c r="BB5" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_10]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_10]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_10]]+1,"")</f>
         <v/>
       </c>
-      <c r="BB5" s="36" t="str">
+      <c r="BD5" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_11]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_11]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_11]]+1,"")</f>
         <v/>
       </c>
-      <c r="BD5" s="36" t="str">
+      <c r="BF5" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_12]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_12]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_12]]+1,"")</f>
         <v/>
       </c>
-      <c r="BF5" s="36" t="str">
+      <c r="BH5" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_13]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_13]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_13]]+1,"")</f>
         <v/>
       </c>
-      <c r="BH5" s="24"/>
-    </row>
-    <row r="6" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="BJ5" s="24"/>
+    </row>
+    <row r="6" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B6" s="24">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="M6" t="s">
+      <c r="K6"/>
+      <c r="M6" s="28"/>
+      <c r="O6" t="s">
         <v>45</v>
       </c>
-      <c r="O6" t="s">
+      <c r="Q6" t="s">
         <v>76</v>
       </c>
-      <c r="AC6" s="25" t="s">
+      <c r="U6"/>
+      <c r="W6" s="28"/>
+      <c r="AC6"/>
+      <c r="AD6"/>
+      <c r="AE6" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="AF6" s="36"/>
-      <c r="AG6" t="s">
+      <c r="AF6" s="24"/>
+      <c r="AH6" s="36"/>
+      <c r="AI6" t="s">
         <v>39</v>
       </c>
-      <c r="AH6" s="36" t="str">
+      <c r="AJ6" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_01]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_01]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_01]]+1,"")</f>
         <v/>
       </c>
-      <c r="AJ6" s="36" t="str">
+      <c r="AL6" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_02]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_02]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_02]]+1,"")</f>
         <v/>
       </c>
-      <c r="AL6" s="36" t="str">
+      <c r="AN6" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_03]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_03]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_03]]+1,"")</f>
         <v/>
       </c>
-      <c r="AN6" s="36" t="str">
+      <c r="AP6" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_04]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_04]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_04]]+1,"")</f>
         <v/>
       </c>
-      <c r="AP6" s="36" t="str">
+      <c r="AR6" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_05]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_05]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_05]]+1,"")</f>
         <v/>
       </c>
-      <c r="AR6" s="36" t="str">
+      <c r="AT6" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_06]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_06]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_06]]+1,"")</f>
         <v/>
       </c>
-      <c r="AT6" s="36" t="str">
+      <c r="AV6" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_07]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_07]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_07]]+1,"")</f>
         <v/>
       </c>
-      <c r="AV6" s="36" t="str">
+      <c r="AX6" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_08]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_08]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_08]]+1,"")</f>
         <v/>
       </c>
-      <c r="AX6" s="36" t="str">
+      <c r="AZ6" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_09]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_09]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_09]]+1,"")</f>
         <v/>
       </c>
-      <c r="AZ6" s="36" t="str">
+      <c r="BB6" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_10]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_10]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_10]]+1,"")</f>
         <v/>
       </c>
-      <c r="BB6" s="36" t="str">
+      <c r="BD6" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_11]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_11]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_11]]+1,"")</f>
         <v/>
       </c>
-      <c r="BD6" s="36" t="str">
+      <c r="BF6" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_12]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_12]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_12]]+1,"")</f>
         <v/>
       </c>
-      <c r="BF6" s="36" t="str">
+      <c r="BH6" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_13]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_13]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_13]]+1,"")</f>
         <v/>
       </c>
-      <c r="BH6" s="24"/>
-    </row>
-    <row r="7" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="BJ6" s="24"/>
+    </row>
+    <row r="7" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B7" s="24">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="M7" t="s">
+      <c r="K7"/>
+      <c r="M7" s="28"/>
+      <c r="O7" t="s">
         <v>46</v>
       </c>
-      <c r="O7" t="s">
+      <c r="Q7" t="s">
         <v>71</v>
       </c>
-      <c r="AC7" s="25" t="s">
+      <c r="U7"/>
+      <c r="W7" s="28"/>
+      <c r="AC7"/>
+      <c r="AD7"/>
+      <c r="AE7" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="AF7" s="36"/>
-      <c r="AG7" t="s">
+      <c r="AF7" s="24"/>
+      <c r="AH7" s="36"/>
+      <c r="AI7" t="s">
         <v>40</v>
       </c>
-      <c r="AH7" s="36" t="str">
+      <c r="AJ7" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_01]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_01]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_01]]+1,"")</f>
         <v/>
       </c>
-      <c r="AJ7" s="36" t="str">
+      <c r="AL7" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_02]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_02]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_02]]+1,"")</f>
         <v/>
       </c>
-      <c r="AL7" s="36" t="str">
+      <c r="AN7" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_03]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_03]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_03]]+1,"")</f>
         <v/>
       </c>
-      <c r="AN7" s="36" t="str">
+      <c r="AP7" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_04]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_04]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_04]]+1,"")</f>
         <v/>
       </c>
-      <c r="AP7" s="36" t="str">
+      <c r="AR7" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_05]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_05]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_05]]+1,"")</f>
         <v/>
       </c>
-      <c r="AR7" s="36" t="str">
+      <c r="AT7" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_06]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_06]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_06]]+1,"")</f>
         <v/>
       </c>
-      <c r="AT7" s="36" t="str">
+      <c r="AV7" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_07]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_07]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_07]]+1,"")</f>
         <v/>
       </c>
-      <c r="AV7" s="36" t="str">
+      <c r="AX7" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_08]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_08]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_08]]+1,"")</f>
         <v/>
       </c>
-      <c r="AX7" s="36" t="str">
+      <c r="AZ7" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_09]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_09]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_09]]+1,"")</f>
         <v/>
       </c>
-      <c r="AZ7" s="36" t="str">
+      <c r="BB7" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_10]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_10]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_10]]+1,"")</f>
         <v/>
       </c>
-      <c r="BB7" s="36" t="str">
+      <c r="BD7" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_11]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_11]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_11]]+1,"")</f>
         <v/>
       </c>
-      <c r="BD7" s="36" t="str">
+      <c r="BF7" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_12]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_12]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_12]]+1,"")</f>
         <v/>
       </c>
-      <c r="BF7" s="36" t="str">
+      <c r="BH7" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_13]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_13]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_13]]+1,"")</f>
         <v/>
       </c>
-      <c r="BH7" s="24"/>
-    </row>
-    <row r="8" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="BJ7" s="24"/>
+    </row>
+    <row r="8" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B8" s="24">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M8" t="s">
+      <c r="K8"/>
+      <c r="M8" s="28"/>
+      <c r="O8" t="s">
         <v>85</v>
       </c>
-      <c r="AC8" s="25" t="s">
+      <c r="U8"/>
+      <c r="W8" s="28"/>
+      <c r="AC8"/>
+      <c r="AD8"/>
+      <c r="AE8" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="AF8" s="36"/>
-      <c r="AG8" t="s">
+      <c r="AF8" s="24"/>
+      <c r="AH8" s="36"/>
+      <c r="AI8" t="s">
         <v>41</v>
       </c>
-      <c r="AH8" s="36" t="str">
+      <c r="AJ8" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_01]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_01]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_01]]+1,"")</f>
         <v/>
       </c>
-      <c r="AJ8" s="36" t="str">
+      <c r="AL8" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_02]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_02]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_02]]+1,"")</f>
         <v/>
       </c>
-      <c r="AL8" s="36" t="str">
+      <c r="AN8" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_03]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_03]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_03]]+1,"")</f>
         <v/>
       </c>
-      <c r="AN8" s="36" t="str">
+      <c r="AP8" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_04]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_04]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_04]]+1,"")</f>
         <v/>
       </c>
-      <c r="AP8" s="36" t="str">
+      <c r="AR8" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_05]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_05]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_05]]+1,"")</f>
         <v/>
       </c>
-      <c r="AR8" s="36" t="str">
+      <c r="AT8" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_06]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_06]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_06]]+1,"")</f>
         <v/>
       </c>
-      <c r="AT8" s="36" t="str">
+      <c r="AV8" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_07]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_07]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_07]]+1,"")</f>
         <v/>
       </c>
-      <c r="AV8" s="36" t="str">
+      <c r="AX8" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_08]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_08]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_08]]+1,"")</f>
         <v/>
       </c>
-      <c r="AX8" s="36" t="str">
+      <c r="AZ8" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_09]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_09]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_09]]+1,"")</f>
         <v/>
       </c>
-      <c r="AZ8" s="36" t="str">
+      <c r="BB8" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_10]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_10]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_10]]+1,"")</f>
         <v/>
       </c>
-      <c r="BB8" s="36" t="str">
+      <c r="BD8" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_11]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_11]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_11]]+1,"")</f>
         <v/>
       </c>
-      <c r="BD8" s="36" t="str">
+      <c r="BF8" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_12]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_12]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_12]]+1,"")</f>
         <v/>
       </c>
-      <c r="BF8" s="36" t="str">
+      <c r="BH8" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_13]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_13]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_13]]+1,"")</f>
         <v/>
       </c>
-      <c r="BH8" s="24"/>
-    </row>
-    <row r="9" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="BJ8" s="24"/>
+    </row>
+    <row r="9" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B9" s="24">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="M9" t="s">
+      <c r="K9"/>
+      <c r="M9" s="28"/>
+      <c r="O9" t="s">
         <v>47</v>
       </c>
-      <c r="AC9" s="25" t="s">
+      <c r="U9"/>
+      <c r="W9" s="28"/>
+      <c r="AC9"/>
+      <c r="AD9"/>
+      <c r="AE9" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="AF9" s="36"/>
-      <c r="AG9" t="s">
+      <c r="AF9" s="24"/>
+      <c r="AH9" s="36"/>
+      <c r="AI9" t="s">
         <v>42</v>
       </c>
-      <c r="AH9" s="36" t="str">
+      <c r="AJ9" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_01]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_01]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_01]]+1,"")</f>
         <v/>
       </c>
-      <c r="AJ9" s="36" t="str">
+      <c r="AL9" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_02]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_02]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_02]]+1,"")</f>
         <v/>
       </c>
-      <c r="AL9" s="36" t="str">
+      <c r="AN9" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_03]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_03]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_03]]+1,"")</f>
         <v/>
       </c>
-      <c r="AN9" s="36" t="str">
+      <c r="AP9" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_04]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_04]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_04]]+1,"")</f>
         <v/>
       </c>
-      <c r="AP9" s="36" t="str">
+      <c r="AR9" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_05]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_05]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_05]]+1,"")</f>
         <v/>
       </c>
-      <c r="AR9" s="36" t="str">
+      <c r="AT9" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_06]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_06]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_06]]+1,"")</f>
         <v/>
       </c>
-      <c r="AT9" s="36" t="str">
+      <c r="AV9" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_07]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_07]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_07]]+1,"")</f>
         <v/>
       </c>
-      <c r="AV9" s="36" t="str">
+      <c r="AX9" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_08]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_08]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_08]]+1,"")</f>
         <v/>
       </c>
-      <c r="AX9" s="36" t="str">
+      <c r="AZ9" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_09]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_09]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_09]]+1,"")</f>
         <v/>
       </c>
-      <c r="AZ9" s="36" t="str">
+      <c r="BB9" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_10]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_10]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_10]]+1,"")</f>
         <v/>
       </c>
-      <c r="BB9" s="36" t="str">
+      <c r="BD9" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_11]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_11]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_11]]+1,"")</f>
         <v/>
       </c>
-      <c r="BD9" s="36" t="str">
+      <c r="BF9" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_12]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_12]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_12]]+1,"")</f>
         <v/>
       </c>
-      <c r="BF9" s="36" t="str">
+      <c r="BH9" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_13]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_13]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_13]]+1,"")</f>
         <v/>
       </c>
-      <c r="BH9" s="24"/>
-    </row>
-    <row r="10" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="BJ9" s="24"/>
+    </row>
+    <row r="10" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B10" s="24">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M10" t="s">
+      <c r="K10"/>
+      <c r="M10" s="28"/>
+      <c r="O10" t="s">
         <v>48</v>
       </c>
-      <c r="AC10" s="25" t="s">
+      <c r="U10"/>
+      <c r="W10" s="28"/>
+      <c r="AC10"/>
+      <c r="AD10"/>
+      <c r="AE10" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="AF10" s="36"/>
-      <c r="AH10" s="36" t="str">
+      <c r="AF10" s="24"/>
+      <c r="AH10" s="36"/>
+      <c r="AJ10" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_01]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_01]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_01]]+1,"")</f>
         <v/>
       </c>
-      <c r="AJ10" s="36" t="str">
+      <c r="AL10" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_02]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_02]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_02]]+1,"")</f>
         <v/>
       </c>
-      <c r="AL10" s="36" t="str">
+      <c r="AN10" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_03]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_03]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_03]]+1,"")</f>
         <v/>
       </c>
-      <c r="AN10" s="36" t="str">
+      <c r="AP10" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_04]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_04]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_04]]+1,"")</f>
         <v/>
       </c>
-      <c r="AP10" s="36" t="str">
+      <c r="AR10" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_05]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_05]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_05]]+1,"")</f>
         <v/>
       </c>
-      <c r="AR10" s="36" t="str">
+      <c r="AT10" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_06]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_06]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_06]]+1,"")</f>
         <v/>
       </c>
-      <c r="AT10" s="36" t="str">
+      <c r="AV10" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_07]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_07]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_07]]+1,"")</f>
         <v/>
       </c>
-      <c r="AV10" s="36" t="str">
+      <c r="AX10" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_08]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_08]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_08]]+1,"")</f>
         <v/>
       </c>
-      <c r="AX10" s="36" t="str">
+      <c r="AZ10" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_09]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_09]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_09]]+1,"")</f>
         <v/>
       </c>
-      <c r="AZ10" s="36" t="str">
+      <c r="BB10" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_10]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_10]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_10]]+1,"")</f>
         <v/>
       </c>
-      <c r="BB10" s="36" t="str">
+      <c r="BD10" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_11]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_11]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_11]]+1,"")</f>
         <v/>
       </c>
-      <c r="BD10" s="36" t="str">
+      <c r="BF10" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_12]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_12]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_12]]+1,"")</f>
         <v/>
       </c>
-      <c r="BF10" s="36" t="str">
+      <c r="BH10" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_13]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_13]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_13]]+1,"")</f>
         <v/>
       </c>
-      <c r="BH10" s="24"/>
-    </row>
-    <row r="11" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="BJ10" s="24"/>
+    </row>
+    <row r="11" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B11" s="24">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="M11" t="s">
+      <c r="K11"/>
+      <c r="M11" s="28"/>
+      <c r="O11" t="s">
         <v>49</v>
       </c>
-      <c r="AC11" s="25" t="s">
+      <c r="U11"/>
+      <c r="W11" s="28"/>
+      <c r="AC11"/>
+      <c r="AD11"/>
+      <c r="AE11" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="AF11" s="36"/>
-      <c r="AH11" s="36" t="str">
+      <c r="AF11" s="24"/>
+      <c r="AH11" s="36"/>
+      <c r="AJ11" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_01]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_01]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_01]]+1,"")</f>
         <v/>
       </c>
-      <c r="AJ11" s="36" t="str">
+      <c r="AL11" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_02]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_02]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_02]]+1,"")</f>
         <v/>
       </c>
-      <c r="AL11" s="36" t="str">
+      <c r="AN11" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_03]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_03]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_03]]+1,"")</f>
         <v/>
       </c>
-      <c r="AN11" s="36" t="str">
+      <c r="AP11" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_04]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_04]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_04]]+1,"")</f>
         <v/>
       </c>
-      <c r="AP11" s="36" t="str">
+      <c r="AR11" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_05]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_05]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_05]]+1,"")</f>
         <v/>
       </c>
-      <c r="AR11" s="36" t="str">
+      <c r="AT11" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_06]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_06]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_06]]+1,"")</f>
         <v/>
       </c>
-      <c r="AT11" s="36" t="str">
+      <c r="AV11" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_07]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_07]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_07]]+1,"")</f>
         <v/>
       </c>
-      <c r="AV11" s="36" t="str">
+      <c r="AX11" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_08]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_08]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_08]]+1,"")</f>
         <v/>
       </c>
-      <c r="AX11" s="36" t="str">
+      <c r="AZ11" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_09]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_09]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_09]]+1,"")</f>
         <v/>
       </c>
-      <c r="AZ11" s="36" t="str">
+      <c r="BB11" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_10]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_10]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_10]]+1,"")</f>
         <v/>
       </c>
-      <c r="BB11" s="36" t="str">
+      <c r="BD11" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_11]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_11]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_11]]+1,"")</f>
         <v/>
       </c>
-      <c r="BD11" s="36" t="str">
+      <c r="BF11" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_12]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_12]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_12]]+1,"")</f>
         <v/>
       </c>
-      <c r="BF11" s="36" t="str">
+      <c r="BH11" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_13]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_13]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_13]]+1,"")</f>
         <v/>
       </c>
-      <c r="BH11" s="24"/>
-    </row>
-    <row r="12" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="BJ11" s="24"/>
+    </row>
+    <row r="12" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B12" s="24">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="M12" t="s">
+      <c r="K12"/>
+      <c r="M12" s="28"/>
+      <c r="O12" t="s">
         <v>50</v>
       </c>
-      <c r="AC12" s="25" t="s">
+      <c r="U12"/>
+      <c r="W12" s="28"/>
+      <c r="AC12"/>
+      <c r="AD12"/>
+      <c r="AE12" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="AF12" s="36"/>
-      <c r="AH12" s="36" t="str">
+      <c r="AF12" s="24"/>
+      <c r="AH12" s="36"/>
+      <c r="AJ12" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_01]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_01]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_01]]+1,"")</f>
         <v/>
       </c>
-      <c r="AJ12" s="36" t="str">
+      <c r="AL12" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_02]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_02]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_02]]+1,"")</f>
         <v/>
       </c>
-      <c r="AL12" s="36" t="str">
+      <c r="AN12" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_03]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_03]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_03]]+1,"")</f>
         <v/>
       </c>
-      <c r="AN12" s="36" t="str">
+      <c r="AP12" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_04]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_04]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_04]]+1,"")</f>
         <v/>
       </c>
-      <c r="AP12" s="36" t="str">
+      <c r="AR12" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_05]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_05]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_05]]+1,"")</f>
         <v/>
       </c>
-      <c r="AR12" s="36" t="str">
+      <c r="AT12" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_06]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_06]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_06]]+1,"")</f>
         <v/>
       </c>
-      <c r="AT12" s="36" t="str">
+      <c r="AV12" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_07]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_07]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_07]]+1,"")</f>
         <v/>
       </c>
-      <c r="AV12" s="36" t="str">
+      <c r="AX12" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_08]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_08]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_08]]+1,"")</f>
         <v/>
       </c>
-      <c r="AX12" s="36" t="str">
+      <c r="AZ12" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_09]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_09]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_09]]+1,"")</f>
         <v/>
       </c>
-      <c r="AZ12" s="36" t="str">
+      <c r="BB12" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_10]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_10]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_10]]+1,"")</f>
         <v/>
       </c>
-      <c r="BB12" s="36" t="str">
+      <c r="BD12" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_11]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_11]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_11]]+1,"")</f>
         <v/>
       </c>
-      <c r="BD12" s="36" t="str">
+      <c r="BF12" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_12]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_12]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_12]]+1,"")</f>
         <v/>
       </c>
-      <c r="BF12" s="36" t="str">
+      <c r="BH12" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_13]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_13]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_13]]+1,"")</f>
         <v/>
       </c>
-      <c r="BH12" s="24"/>
-    </row>
-    <row r="13" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="BJ12" s="24"/>
+    </row>
+    <row r="13" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B13" s="24">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="M13" t="s">
+      <c r="K13"/>
+      <c r="M13" s="28"/>
+      <c r="O13" t="s">
         <v>51</v>
       </c>
-      <c r="AC13" s="25" t="s">
+      <c r="U13"/>
+      <c r="W13" s="28"/>
+      <c r="AC13"/>
+      <c r="AD13"/>
+      <c r="AE13" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="AF13" s="36"/>
-      <c r="AH13" s="36" t="str">
+      <c r="AF13" s="24"/>
+      <c r="AH13" s="36"/>
+      <c r="AJ13" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_01]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_01]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_01]]+1,"")</f>
         <v/>
       </c>
-      <c r="AJ13" s="36" t="str">
+      <c r="AL13" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_02]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_02]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_02]]+1,"")</f>
         <v/>
       </c>
-      <c r="AL13" s="36" t="str">
+      <c r="AN13" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_03]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_03]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_03]]+1,"")</f>
         <v/>
       </c>
-      <c r="AN13" s="36" t="str">
+      <c r="AP13" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_04]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_04]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_04]]+1,"")</f>
         <v/>
       </c>
-      <c r="AP13" s="36" t="str">
+      <c r="AR13" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_05]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_05]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_05]]+1,"")</f>
         <v/>
       </c>
-      <c r="AR13" s="36" t="str">
+      <c r="AT13" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_06]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_06]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_06]]+1,"")</f>
         <v/>
       </c>
-      <c r="AT13" s="36" t="str">
+      <c r="AV13" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_07]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_07]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_07]]+1,"")</f>
         <v/>
       </c>
-      <c r="AV13" s="36" t="str">
+      <c r="AX13" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_08]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_08]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_08]]+1,"")</f>
         <v/>
       </c>
-      <c r="AX13" s="36" t="str">
+      <c r="AZ13" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_09]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_09]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_09]]+1,"")</f>
         <v/>
       </c>
-      <c r="AZ13" s="36" t="str">
+      <c r="BB13" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_10]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_10]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_10]]+1,"")</f>
         <v/>
       </c>
-      <c r="BB13" s="36" t="str">
+      <c r="BD13" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_11]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_11]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_11]]+1,"")</f>
         <v/>
       </c>
-      <c r="BD13" s="36" t="str">
+      <c r="BF13" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_12]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_12]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_12]]+1,"")</f>
         <v/>
       </c>
-      <c r="BF13" s="36" t="str">
+      <c r="BH13" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_13]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_13]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_13]]+1,"")</f>
         <v/>
       </c>
-      <c r="BH13" s="24"/>
-    </row>
-    <row r="14" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="BJ13" s="24"/>
+    </row>
+    <row r="14" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B14" s="24">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M14" t="s">
+      <c r="K14"/>
+      <c r="M14" s="28"/>
+      <c r="O14" t="s">
         <v>52</v>
       </c>
-      <c r="AC14" s="25" t="s">
+      <c r="U14"/>
+      <c r="W14" s="28"/>
+      <c r="AC14"/>
+      <c r="AD14"/>
+      <c r="AE14" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="AF14" s="36"/>
-      <c r="AH14" s="36" t="str">
+      <c r="AF14" s="24"/>
+      <c r="AH14" s="36"/>
+      <c r="AJ14" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_01]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_01]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_01]]+1,"")</f>
         <v/>
       </c>
-      <c r="AJ14" s="36" t="str">
+      <c r="AL14" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_02]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_02]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_02]]+1,"")</f>
         <v/>
       </c>
-      <c r="AL14" s="36" t="str">
+      <c r="AN14" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_03]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_03]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_03]]+1,"")</f>
         <v/>
       </c>
-      <c r="AN14" s="36" t="str">
+      <c r="AP14" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_04]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_04]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_04]]+1,"")</f>
         <v/>
       </c>
-      <c r="AP14" s="36" t="str">
+      <c r="AR14" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_05]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_05]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_05]]+1,"")</f>
         <v/>
       </c>
-      <c r="AR14" s="36" t="str">
+      <c r="AT14" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_06]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_06]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_06]]+1,"")</f>
         <v/>
       </c>
-      <c r="AT14" s="36" t="str">
+      <c r="AV14" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_07]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_07]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_07]]+1,"")</f>
         <v/>
       </c>
-      <c r="AV14" s="36" t="str">
+      <c r="AX14" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_08]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_08]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_08]]+1,"")</f>
         <v/>
       </c>
-      <c r="AX14" s="36" t="str">
+      <c r="AZ14" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_09]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_09]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_09]]+1,"")</f>
         <v/>
       </c>
-      <c r="AZ14" s="36" t="str">
+      <c r="BB14" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_10]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_10]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_10]]+1,"")</f>
         <v/>
       </c>
-      <c r="BB14" s="36" t="str">
+      <c r="BD14" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_11]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_11]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_11]]+1,"")</f>
         <v/>
       </c>
-      <c r="BD14" s="36" t="str">
+      <c r="BF14" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_12]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_12]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_12]]+1,"")</f>
         <v/>
       </c>
-      <c r="BF14" s="36" t="str">
+      <c r="BH14" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_13]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_13]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_13]]+1,"")</f>
         <v/>
       </c>
-      <c r="BH14" s="24"/>
-    </row>
-    <row r="15" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="BJ14" s="24"/>
+    </row>
+    <row r="15" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B15" s="24">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="M15" t="s">
+      <c r="K15"/>
+      <c r="M15" s="28"/>
+      <c r="O15" t="s">
         <v>53</v>
       </c>
-      <c r="AC15" s="25" t="s">
+      <c r="U15"/>
+      <c r="W15" s="28"/>
+      <c r="AC15"/>
+      <c r="AD15"/>
+      <c r="AE15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="AF15" s="36"/>
-      <c r="AH15" s="36" t="str">
+      <c r="AF15" s="24"/>
+      <c r="AH15" s="36"/>
+      <c r="AJ15" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_01]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_01]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_01]]+1,"")</f>
         <v/>
       </c>
-      <c r="AJ15" s="36" t="str">
+      <c r="AL15" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_02]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_02]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_02]]+1,"")</f>
         <v/>
       </c>
-      <c r="AL15" s="36" t="str">
+      <c r="AN15" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_03]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_03]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_03]]+1,"")</f>
         <v/>
       </c>
-      <c r="AN15" s="36" t="str">
+      <c r="AP15" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_04]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_04]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_04]]+1,"")</f>
         <v/>
       </c>
-      <c r="AP15" s="36" t="str">
+      <c r="AR15" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_05]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_05]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_05]]+1,"")</f>
         <v/>
       </c>
-      <c r="AR15" s="36" t="str">
+      <c r="AT15" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_06]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_06]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_06]]+1,"")</f>
         <v/>
       </c>
-      <c r="AT15" s="36" t="str">
+      <c r="AV15" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_07]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_07]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_07]]+1,"")</f>
         <v/>
       </c>
-      <c r="AV15" s="36" t="str">
+      <c r="AX15" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_08]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_08]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_08]]+1,"")</f>
         <v/>
       </c>
-      <c r="AX15" s="36" t="str">
+      <c r="AZ15" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_09]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_09]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_09]]+1,"")</f>
         <v/>
       </c>
-      <c r="AZ15" s="36" t="str">
+      <c r="BB15" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_10]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_10]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_10]]+1,"")</f>
         <v/>
       </c>
-      <c r="BB15" s="36" t="str">
+      <c r="BD15" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_11]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_11]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_11]]+1,"")</f>
         <v/>
       </c>
-      <c r="BD15" s="36" t="str">
+      <c r="BF15" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_12]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_12]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_12]]+1,"")</f>
         <v/>
       </c>
-      <c r="BF15" s="36" t="str">
+      <c r="BH15" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_13]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_13]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_13]]+1,"")</f>
         <v/>
       </c>
-      <c r="BH15" s="24"/>
-    </row>
-    <row r="16" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="BJ15" s="24"/>
+    </row>
+    <row r="16" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B16" s="24">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="M16" t="s">
+      <c r="K16"/>
+      <c r="M16" s="28"/>
+      <c r="O16" t="s">
         <v>54</v>
       </c>
-      <c r="AC16" s="25" t="s">
+      <c r="U16"/>
+      <c r="W16" s="28"/>
+      <c r="AC16"/>
+      <c r="AD16"/>
+      <c r="AE16" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="AF16" s="36"/>
-      <c r="AH16" s="36" t="str">
+      <c r="AF16" s="24"/>
+      <c r="AH16" s="36"/>
+      <c r="AJ16" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_01]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_01]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_01]]+1,"")</f>
         <v/>
       </c>
-      <c r="AJ16" s="36" t="str">
+      <c r="AL16" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_02]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_02]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_02]]+1,"")</f>
         <v/>
       </c>
-      <c r="AL16" s="36" t="str">
+      <c r="AN16" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_03]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_03]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_03]]+1,"")</f>
         <v/>
       </c>
-      <c r="AN16" s="36" t="str">
+      <c r="AP16" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_04]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_04]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_04]]+1,"")</f>
         <v/>
       </c>
-      <c r="AP16" s="36" t="str">
+      <c r="AR16" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_05]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_05]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_05]]+1,"")</f>
         <v/>
       </c>
-      <c r="AR16" s="36" t="str">
+      <c r="AT16" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_06]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_06]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_06]]+1,"")</f>
         <v/>
       </c>
-      <c r="AT16" s="36" t="str">
+      <c r="AV16" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_07]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_07]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_07]]+1,"")</f>
         <v/>
       </c>
-      <c r="AV16" s="36" t="str">
+      <c r="AX16" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_08]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_08]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_08]]+1,"")</f>
         <v/>
       </c>
-      <c r="AX16" s="36" t="str">
+      <c r="AZ16" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_09]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_09]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_09]]+1,"")</f>
         <v/>
       </c>
-      <c r="AZ16" s="36" t="str">
+      <c r="BB16" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_10]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_10]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_10]]+1,"")</f>
         <v/>
       </c>
-      <c r="BB16" s="36" t="str">
+      <c r="BD16" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_11]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_11]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_11]]+1,"")</f>
         <v/>
       </c>
-      <c r="BD16" s="36" t="str">
+      <c r="BF16" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_12]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_12]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_12]]+1,"")</f>
         <v/>
       </c>
-      <c r="BF16" s="36" t="str">
+      <c r="BH16" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_13]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_13]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_13]]+1,"")</f>
         <v/>
       </c>
-      <c r="BH16" s="24"/>
-    </row>
-    <row r="17" spans="2:58" x14ac:dyDescent="0.25">
+      <c r="BJ16" s="24"/>
+    </row>
+    <row r="17" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B17" s="24">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="AC17" s="25" t="s">
+      <c r="K17"/>
+      <c r="M17" s="28"/>
+      <c r="U17"/>
+      <c r="W17" s="28"/>
+      <c r="AC17"/>
+      <c r="AD17"/>
+      <c r="AE17" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="AF17" s="36"/>
-      <c r="AH17" s="36" t="str">
+      <c r="AF17" s="24"/>
+      <c r="AH17" s="36"/>
+      <c r="AJ17" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_01]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_01]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_01]]+1,"")</f>
         <v/>
       </c>
-      <c r="AJ17" s="36" t="str">
+      <c r="AL17" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_02]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_02]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_02]]+1,"")</f>
         <v/>
       </c>
-      <c r="AL17" s="36" t="str">
+      <c r="AN17" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_03]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_03]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_03]]+1,"")</f>
         <v/>
       </c>
-      <c r="AN17" s="36" t="str">
+      <c r="AP17" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_04]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_04]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_04]]+1,"")</f>
         <v/>
       </c>
-      <c r="AP17" s="36" t="str">
+      <c r="AR17" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_05]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_05]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_05]]+1,"")</f>
         <v/>
       </c>
-      <c r="AR17" s="36" t="str">
+      <c r="AT17" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_06]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_06]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_06]]+1,"")</f>
         <v/>
       </c>
-      <c r="AT17" s="36" t="str">
+      <c r="AV17" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_07]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_07]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_07]]+1,"")</f>
         <v/>
       </c>
-      <c r="AV17" s="36" t="str">
+      <c r="AX17" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_08]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_08]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_08]]+1,"")</f>
         <v/>
       </c>
-      <c r="AX17" s="36" t="str">
+      <c r="AZ17" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_09]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_09]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_09]]+1,"")</f>
         <v/>
       </c>
-      <c r="AZ17" s="36" t="str">
+      <c r="BB17" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_10]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_10]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_10]]+1,"")</f>
         <v/>
       </c>
-      <c r="BB17" s="36" t="str">
+      <c r="BD17" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_11]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_11]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_11]]+1,"")</f>
         <v/>
       </c>
-      <c r="BD17" s="36" t="str">
+      <c r="BF17" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_12]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_12]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_12]]+1,"")</f>
         <v/>
       </c>
-      <c r="BF17" s="36" t="str">
+      <c r="BH17" s="36" t="str">
         <f>IF(AND(Table8[[#This Row],[tulemus_13]]&lt;&gt;"",ISNUMBER(DATEVALUE(TEXT(Table8[[#This Row],[kuupäev_13]],"dd.mm.yyyy")))),Table8[[#This Row],[kuupäev_13]]+1,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="2:58" x14ac:dyDescent="0.25">
+      <c r="BJ17" s="28"/>
+    </row>
+    <row r="18" spans="2:62" x14ac:dyDescent="0.25">
       <c r="AC18" s="25"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="J2">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(H2))=0</formula>
+      <formula>LEN(TRIM(J2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="18">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+  <dataValidations count="20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
       <formula1>"N, M, Teadmata"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Kui kontaktne osutus positiivseks, siis siia kirja panna positiivse unikaalne number (tabelist COVID19_2020 KOONDTABEL)." sqref="U1:V1"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Lisa esmase kahtlusaluse unikaalne ID (&amp; nimi) kõigile tema kontaktsetele." sqref="L1"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G17">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Kui kontaktne osutus positiivseks, siis siia kirja panna positiivse unikaalne number (tabelist COVID19_2020 KOONDTABEL)." sqref="W1:X1"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Lisa esmase kahtlusaluse unikaalne ID (&amp; nimi) kõigile tema kontaktsetele." sqref="N1"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I17">
       <formula1>Lists_Sugu</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M17">
       <formula1>Lists_Kontakti_tüüp</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O3:O17">
       <formula1>Lists_Kontakti_koht</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O3:O17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q3:Q17">
       <formula1>Lists_Elukutse</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q3:Q17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S3:S17">
       <formula1>Lists_Riskipiirkonnas_viibimine</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC3:AC17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE3:AE17">
       <formula1>Lists_Peamised_sümptomid</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG3:AG17 AI3:AI17 AK3:AK17 AM3:AM17 AO3:AO17 AQ3:AQ17 AS3:AS17 AU3:AU17 AW3:AW17 AY3:AY17 BA3:BA17 BC3:BC17 BE3:BE17 BG3:BG17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI3:AI17 AK3:AK17 AM3:AM17 AO3:AO17 AQ3:AQ17 AS3:AS17 AU3:AU17 AW3:AW17 AY3:AY17 BA3:BA17 BC3:BC17 BE3:BE17 BG3:BG17 BI3:BI17">
       <formula1>Lists_Tulemus</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Vanus" error="Suggested to enter as number between 1 and 100" sqref="H3:H17">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Vanus" error="Suggested to enter as number between 1 and 100" sqref="J3:J17">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="E-post" error="Please enter valid email" sqref="I3:I17">
-      <formula1>ISNUMBER(MATCH("*@*.?*",I3,0))</formula1>
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="E-post" error="Please enter valid email" sqref="K3:K17">
+      <formula1>ISNUMBER(MATCH("*@*.?*",K3,0))</formula1>
     </dataValidation>
-    <dataValidation type="date" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Kontakti viimane kpv" error="Please enter the date between  Minimum_Kontakti_viimane_kpv and Maximum_Kontakti_viimane_kpv" sqref="P3:P17">
+    <dataValidation type="date" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Kontakti viimane kpv" error="Please enter the date between  Minimum_Kontakti_viimane_kpv and Maximum_Kontakti_viimane_kpv" sqref="R3:R17">
       <formula1>Minimum_Kontakti_viimane_kpv</formula1>
       <formula2>Maximum_Kontakti_viimane_kpv</formula2>
     </dataValidation>
-    <dataValidation type="date" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Kontakti viimane kpv" error="Please enter the date between  Minimum_Eestisse_Saabumise_kpv and Maximum_Eestisse_Saabumise_kpv " sqref="T3:T17">
+    <dataValidation type="date" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Kontakti viimane kpv" error="Please enter the date between  Minimum_Eestisse_Saabumise_kpv and Maximum_Eestisse_Saabumise_kpv " sqref="V3:V17">
       <formula1>Minimum_Eestisse_saabumise_kpv</formula1>
       <formula2>Maximum_Eestisse_saabumise_kpv</formula2>
     </dataValidation>
-    <dataValidation type="date" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Kontakti viimane kpv" error="Please enter the date between  Minimum_Esimeste_haigusnähtude_ilmumise_kuupäev and Maximum_Esimeste_haigusnähtude_ilmumise_kuupäev " sqref="AB3:AB17">
+    <dataValidation type="date" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Kontakti viimane kpv" error="Please enter the date between  Minimum_Esimeste_haigusnähtude_ilmumise_kuupäev and Maximum_Esimeste_haigusnähtude_ilmumise_kuupäev " sqref="AD3:AD17">
       <formula1>Minimum_Esimeste_haigusnähtude_ilmumise_kuupäev</formula1>
       <formula2>Maximum_Esimeste_haigusnähtude_ilmumise_kuupäev</formula2>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Temperatuur" error="Please enter Temperatuur between Minimum_Temperatuur and Maximum_Temperatuur" sqref="AD3:AD17">
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Temperatuur" error="Please enter Temperatuur between Minimum_Temperatuur and Maximum_Temperatuur" sqref="AF3:AF17">
       <formula1>Minimum_Temperatuur</formula1>
       <formula2>Maximum_Temperatuur</formula2>
     </dataValidation>
-    <dataValidation type="date" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Jälgimise päev" error="Please enter jälgimise päev between Minimum_Jälgimise_kuupäev and Maximum_Jälgimise_kuupäev" sqref="BF3:BF17 AJ3:AJ17 AL3:AL17 AN3:AN17 AP3:AP17 AR3:AR17 AT3:AT17 AV3:AV17 AX3:AX17 AZ3:AZ17 BB3:BB17 BD3:BD17 AH3:AH17">
+    <dataValidation type="date" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Jälgimise päev" error="Please enter jälgimise päev between Minimum_Jälgimise_kuupäev and Maximum_Jälgimise_kuupäev" sqref="BH3:BH17 AL3:AL17 AN3:AN17 AP3:AP17 AR3:AR17 AT3:AT17 AV3:AV17 AX3:AX17 AZ3:AZ17 BB3:BB17 BD3:BD17 BF3:BF17 AJ3:AJ17">
       <formula1>Minimum_Jälgimise_kuupäev</formula1>
       <formula2>Maximum_Jälgimise_kuupäev</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D17">
       <formula1>Eesti_KOV_Maakond_Vald_Linn</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E17">
+      <formula1>Eesti_KOV_2_Maakond</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F17">
+      <formula1>INDIRECT(SUBSTITUTE(SUBSTITUTE($E3," ","_"),"-","_"))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3760,7 +4042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C53" sqref="C2:C80"/>
     </sheetView>
   </sheetViews>
@@ -4740,11 +5022,852 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="10" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" customWidth="1"/>
+    <col min="14" max="14" width="18.5703125" customWidth="1"/>
+    <col min="15" max="15" width="16" customWidth="1"/>
+    <col min="19" max="19" width="21.5703125" customWidth="1"/>
+    <col min="20" max="20" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J1" t="s">
+        <v>218</v>
+      </c>
+      <c r="K1" t="s">
+        <v>223</v>
+      </c>
+      <c r="L1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M1" t="s">
+        <v>236</v>
+      </c>
+      <c r="N1" t="s">
+        <v>240</v>
+      </c>
+      <c r="O1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H2" t="s">
+        <v>207</v>
+      </c>
+      <c r="I2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J2" t="s">
+        <v>219</v>
+      </c>
+      <c r="K2" t="s">
+        <v>224</v>
+      </c>
+      <c r="L2" t="s">
+        <v>228</v>
+      </c>
+      <c r="M2" t="s">
+        <v>237</v>
+      </c>
+      <c r="N2" t="s">
+        <v>241</v>
+      </c>
+      <c r="O2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G3" t="s">
+        <v>199</v>
+      </c>
+      <c r="H3" t="s">
+        <v>208</v>
+      </c>
+      <c r="I3" t="s">
+        <v>212</v>
+      </c>
+      <c r="J3" t="s">
+        <v>220</v>
+      </c>
+      <c r="K3" t="s">
+        <v>225</v>
+      </c>
+      <c r="L3" t="s">
+        <v>229</v>
+      </c>
+      <c r="M3" t="s">
+        <v>238</v>
+      </c>
+      <c r="N3" t="s">
+        <v>242</v>
+      </c>
+      <c r="O3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" t="s">
+        <v>263</v>
+      </c>
+      <c r="C4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" t="s">
+        <v>200</v>
+      </c>
+      <c r="H4" t="s">
+        <v>209</v>
+      </c>
+      <c r="I4" t="s">
+        <v>213</v>
+      </c>
+      <c r="J4" t="s">
+        <v>221</v>
+      </c>
+      <c r="K4" t="s">
+        <v>226</v>
+      </c>
+      <c r="L4" t="s">
+        <v>230</v>
+      </c>
+      <c r="M4" t="s">
+        <v>239</v>
+      </c>
+      <c r="N4" t="s">
+        <v>243</v>
+      </c>
+      <c r="O4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" t="s">
+        <v>263</v>
+      </c>
+      <c r="E5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F5" t="s">
+        <v>263</v>
+      </c>
+      <c r="G5" t="s">
+        <v>201</v>
+      </c>
+      <c r="H5" t="s">
+        <v>263</v>
+      </c>
+      <c r="I5" t="s">
+        <v>214</v>
+      </c>
+      <c r="J5" t="s">
+        <v>222</v>
+      </c>
+      <c r="K5" t="s">
+        <v>263</v>
+      </c>
+      <c r="L5" t="s">
+        <v>231</v>
+      </c>
+      <c r="M5" t="s">
+        <v>263</v>
+      </c>
+      <c r="N5" t="s">
+        <v>244</v>
+      </c>
+      <c r="O5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" t="s">
+        <v>263</v>
+      </c>
+      <c r="C6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D6" t="s">
+        <v>263</v>
+      </c>
+      <c r="E6" t="s">
+        <v>263</v>
+      </c>
+      <c r="F6" t="s">
+        <v>263</v>
+      </c>
+      <c r="G6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H6" t="s">
+        <v>263</v>
+      </c>
+      <c r="I6" t="s">
+        <v>215</v>
+      </c>
+      <c r="J6" t="s">
+        <v>263</v>
+      </c>
+      <c r="K6" t="s">
+        <v>263</v>
+      </c>
+      <c r="L6" t="s">
+        <v>232</v>
+      </c>
+      <c r="M6" t="s">
+        <v>263</v>
+      </c>
+      <c r="N6" t="s">
+        <v>263</v>
+      </c>
+      <c r="O6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E7" t="s">
+        <v>263</v>
+      </c>
+      <c r="F7" t="s">
+        <v>263</v>
+      </c>
+      <c r="G7" t="s">
+        <v>203</v>
+      </c>
+      <c r="H7" t="s">
+        <v>263</v>
+      </c>
+      <c r="I7" t="s">
+        <v>216</v>
+      </c>
+      <c r="J7" t="s">
+        <v>263</v>
+      </c>
+      <c r="K7" t="s">
+        <v>263</v>
+      </c>
+      <c r="L7" t="s">
+        <v>233</v>
+      </c>
+      <c r="M7" t="s">
+        <v>263</v>
+      </c>
+      <c r="N7" t="s">
+        <v>263</v>
+      </c>
+      <c r="O7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" t="s">
+        <v>263</v>
+      </c>
+      <c r="C8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E8" t="s">
+        <v>263</v>
+      </c>
+      <c r="F8" t="s">
+        <v>263</v>
+      </c>
+      <c r="G8" t="s">
+        <v>204</v>
+      </c>
+      <c r="H8" t="s">
+        <v>263</v>
+      </c>
+      <c r="I8" t="s">
+        <v>217</v>
+      </c>
+      <c r="J8" t="s">
+        <v>263</v>
+      </c>
+      <c r="K8" t="s">
+        <v>263</v>
+      </c>
+      <c r="L8" t="s">
+        <v>234</v>
+      </c>
+      <c r="M8" t="s">
+        <v>263</v>
+      </c>
+      <c r="N8" t="s">
+        <v>263</v>
+      </c>
+      <c r="O8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" t="s">
+        <v>263</v>
+      </c>
+      <c r="C9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" t="s">
+        <v>263</v>
+      </c>
+      <c r="E9" t="s">
+        <v>263</v>
+      </c>
+      <c r="F9" t="s">
+        <v>263</v>
+      </c>
+      <c r="G9" t="s">
+        <v>205</v>
+      </c>
+      <c r="H9" t="s">
+        <v>263</v>
+      </c>
+      <c r="I9" t="s">
+        <v>263</v>
+      </c>
+      <c r="J9" t="s">
+        <v>263</v>
+      </c>
+      <c r="K9" t="s">
+        <v>263</v>
+      </c>
+      <c r="L9" t="s">
+        <v>235</v>
+      </c>
+      <c r="M9" t="s">
+        <v>263</v>
+      </c>
+      <c r="N9" t="s">
+        <v>263</v>
+      </c>
+      <c r="O9" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10" t="s">
+        <v>263</v>
+      </c>
+      <c r="C10" t="s">
+        <v>263</v>
+      </c>
+      <c r="D10" t="s">
+        <v>263</v>
+      </c>
+      <c r="E10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F10" t="s">
+        <v>263</v>
+      </c>
+      <c r="G10" t="s">
+        <v>263</v>
+      </c>
+      <c r="H10" t="s">
+        <v>263</v>
+      </c>
+      <c r="I10" t="s">
+        <v>263</v>
+      </c>
+      <c r="J10" t="s">
+        <v>263</v>
+      </c>
+      <c r="K10" t="s">
+        <v>263</v>
+      </c>
+      <c r="L10" t="s">
+        <v>263</v>
+      </c>
+      <c r="M10" t="s">
+        <v>263</v>
+      </c>
+      <c r="N10" t="s">
+        <v>263</v>
+      </c>
+      <c r="O10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" t="s">
+        <v>263</v>
+      </c>
+      <c r="C11" t="s">
+        <v>263</v>
+      </c>
+      <c r="D11" t="s">
+        <v>263</v>
+      </c>
+      <c r="E11" t="s">
+        <v>263</v>
+      </c>
+      <c r="F11" t="s">
+        <v>263</v>
+      </c>
+      <c r="G11" t="s">
+        <v>263</v>
+      </c>
+      <c r="H11" t="s">
+        <v>263</v>
+      </c>
+      <c r="I11" t="s">
+        <v>263</v>
+      </c>
+      <c r="J11" t="s">
+        <v>263</v>
+      </c>
+      <c r="K11" t="s">
+        <v>263</v>
+      </c>
+      <c r="L11" t="s">
+        <v>263</v>
+      </c>
+      <c r="M11" t="s">
+        <v>263</v>
+      </c>
+      <c r="N11" t="s">
+        <v>263</v>
+      </c>
+      <c r="O11" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" t="s">
+        <v>263</v>
+      </c>
+      <c r="C12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D12" t="s">
+        <v>263</v>
+      </c>
+      <c r="E12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F12" t="s">
+        <v>263</v>
+      </c>
+      <c r="G12" t="s">
+        <v>263</v>
+      </c>
+      <c r="H12" t="s">
+        <v>263</v>
+      </c>
+      <c r="I12" t="s">
+        <v>263</v>
+      </c>
+      <c r="J12" t="s">
+        <v>263</v>
+      </c>
+      <c r="K12" t="s">
+        <v>263</v>
+      </c>
+      <c r="L12" t="s">
+        <v>263</v>
+      </c>
+      <c r="M12" t="s">
+        <v>263</v>
+      </c>
+      <c r="N12" t="s">
+        <v>263</v>
+      </c>
+      <c r="O12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" t="s">
+        <v>263</v>
+      </c>
+      <c r="C13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D13" t="s">
+        <v>263</v>
+      </c>
+      <c r="E13" t="s">
+        <v>263</v>
+      </c>
+      <c r="F13" t="s">
+        <v>263</v>
+      </c>
+      <c r="G13" t="s">
+        <v>263</v>
+      </c>
+      <c r="H13" t="s">
+        <v>263</v>
+      </c>
+      <c r="I13" t="s">
+        <v>263</v>
+      </c>
+      <c r="J13" t="s">
+        <v>263</v>
+      </c>
+      <c r="K13" t="s">
+        <v>263</v>
+      </c>
+      <c r="L13" t="s">
+        <v>263</v>
+      </c>
+      <c r="M13" t="s">
+        <v>263</v>
+      </c>
+      <c r="N13" t="s">
+        <v>263</v>
+      </c>
+      <c r="O13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C14" t="s">
+        <v>263</v>
+      </c>
+      <c r="D14" t="s">
+        <v>263</v>
+      </c>
+      <c r="E14" t="s">
+        <v>263</v>
+      </c>
+      <c r="F14" t="s">
+        <v>263</v>
+      </c>
+      <c r="G14" t="s">
+        <v>263</v>
+      </c>
+      <c r="H14" t="s">
+        <v>263</v>
+      </c>
+      <c r="I14" t="s">
+        <v>263</v>
+      </c>
+      <c r="J14" t="s">
+        <v>263</v>
+      </c>
+      <c r="K14" t="s">
+        <v>263</v>
+      </c>
+      <c r="L14" t="s">
+        <v>263</v>
+      </c>
+      <c r="M14" t="s">
+        <v>263</v>
+      </c>
+      <c r="N14" t="s">
+        <v>263</v>
+      </c>
+      <c r="O14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B15" t="s">
+        <v>263</v>
+      </c>
+      <c r="C15" t="s">
+        <v>263</v>
+      </c>
+      <c r="D15" t="s">
+        <v>263</v>
+      </c>
+      <c r="E15" t="s">
+        <v>263</v>
+      </c>
+      <c r="F15" t="s">
+        <v>263</v>
+      </c>
+      <c r="G15" t="s">
+        <v>263</v>
+      </c>
+      <c r="H15" t="s">
+        <v>263</v>
+      </c>
+      <c r="I15" t="s">
+        <v>263</v>
+      </c>
+      <c r="J15" t="s">
+        <v>263</v>
+      </c>
+      <c r="K15" t="s">
+        <v>263</v>
+      </c>
+      <c r="L15" t="s">
+        <v>263</v>
+      </c>
+      <c r="M15" t="s">
+        <v>263</v>
+      </c>
+      <c r="N15" t="s">
+        <v>263</v>
+      </c>
+      <c r="O15" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B16" t="s">
+        <v>263</v>
+      </c>
+      <c r="C16" t="s">
+        <v>263</v>
+      </c>
+      <c r="D16" t="s">
+        <v>263</v>
+      </c>
+      <c r="E16" t="s">
+        <v>263</v>
+      </c>
+      <c r="F16" t="s">
+        <v>263</v>
+      </c>
+      <c r="G16" t="s">
+        <v>263</v>
+      </c>
+      <c r="H16" t="s">
+        <v>263</v>
+      </c>
+      <c r="I16" t="s">
+        <v>263</v>
+      </c>
+      <c r="J16" t="s">
+        <v>263</v>
+      </c>
+      <c r="K16" t="s">
+        <v>263</v>
+      </c>
+      <c r="L16" t="s">
+        <v>263</v>
+      </c>
+      <c r="M16" t="s">
+        <v>263</v>
+      </c>
+      <c r="N16" t="s">
+        <v>263</v>
+      </c>
+      <c r="O16" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B17" t="s">
+        <v>263</v>
+      </c>
+      <c r="C17" t="s">
+        <v>263</v>
+      </c>
+      <c r="D17" t="s">
+        <v>263</v>
+      </c>
+      <c r="E17" t="s">
+        <v>263</v>
+      </c>
+      <c r="F17" t="s">
+        <v>263</v>
+      </c>
+      <c r="G17" t="s">
+        <v>263</v>
+      </c>
+      <c r="H17" t="s">
+        <v>263</v>
+      </c>
+      <c r="I17" t="s">
+        <v>263</v>
+      </c>
+      <c r="J17" t="s">
+        <v>263</v>
+      </c>
+      <c r="K17" t="s">
+        <v>263</v>
+      </c>
+      <c r="L17" t="s">
+        <v>263</v>
+      </c>
+      <c r="M17" t="s">
+        <v>263</v>
+      </c>
+      <c r="N17" t="s">
+        <v>263</v>
+      </c>
+      <c r="O17" t="s">
+        <v>263</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S4">
+      <formula1>$A$1:$O$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T4">
+      <formula1>INDIRECT(SUBSTITUTE(SUBSTITUTE($S2," ","_"),"-","_"))</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>